<commit_message>
Create Fundamentals of Electromagnetism Lab Instruction
</commit_message>
<xml_diff>
--- a/111-2/FUNDAMENTALS OF ELECTROMAGNETISM/APP01.xlsx
+++ b/111-2/FUNDAMENTALS OF ELECTROMAGNETISM/APP01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\FCU\111-2\FUNDAMENTALS OF ELECTROMAGNETISM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77B19032-4A1F-499C-8094-108783D41922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95638B2E-E428-400C-B967-1C02B0318D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7D1F19F5-FF57-44EE-A97F-AE46F4CFE104}"/>
   </bookViews>
@@ -128,11 +128,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2392,7 +2392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09EEFB5-E1B8-410C-9729-F801B7EA1DBF}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="97" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -2403,10 +2403,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2469,7 +2469,7 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <f>(E4-E5)/E5</f>
         <v>3.0024169579183711E-2</v>
       </c>
@@ -2499,10 +2499,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2565,7 +2565,7 @@
       <c r="D17" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <f>(E16-E15)/E16</f>
         <v>0.10690310266492553</v>
       </c>

</xml_diff>